<commit_message>
PDS .xls and .csv Files Fixes
Line 58: Filled cell ICON_PATH_DEFAULT with 000-000-000_generic
Line 151: Filled cell #HEX with #D61F82
Line 405: Filled cell ICON_PATH_DEFAULT with 900-9300-000_building
</commit_message>
<xml_diff>
--- a/Carto Icons/POI/PDS_Category_Assignment.xlsx
+++ b/Carto Icons/POI/PDS_Category_Assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lembke/Desktop/HERE/GIT/icons-by-here-technologies/Carto Icons/POI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmcs-my.sharepoint.com/personal/alvaro_lauragarcia_here_com/Documents/GIT/icons-by-here-technologies/Carto Icons/POI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA93A1CC-B8CF-ED45-94D1-7E79B963AF98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{18D1B83F-F0BC-2A47-9648-5D055207C85A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{C64EB798-04F6-AE43-9DCC-0EA02E11247A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34660" windowHeight="27760" xr2:uid="{C64EB798-04F6-AE43-9DCC-0EA02E11247A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="987">
   <si>
     <t>PDS Category name</t>
   </si>
@@ -12034,6 +12034,106 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>404</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>404</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="188" name="Graphic 187">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83BDC2BC-B4C8-9A48-829A-610B7AFD515C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId151">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId152"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18186400" y="256540000"/>
+          <a:ext cx="457200" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="191" name="Graphic 190">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A5460EB-34DF-B64C-A3F5-249DEBD85283}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId34"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18186400" y="36195000"/>
+          <a:ext cx="457200" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12336,8 +12436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693BBA9B-95F3-BD4A-928B-DD81DFE8C409}">
   <dimension ref="A1:I422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="C387" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="50" customHeight="1" outlineLevelCol="1"/>
@@ -13332,7 +13432,9 @@
       <c r="D58" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E58" s="10"/>
+      <c r="E58" s="10" t="s">
+        <v>985</v>
+      </c>
       <c r="F58" s="10"/>
       <c r="G58" s="23" t="s">
         <v>871</v>
@@ -14838,6 +14940,9 @@
         <v>980</v>
       </c>
       <c r="F151" s="10"/>
+      <c r="G151" s="34" t="s">
+        <v>918</v>
+      </c>
     </row>
     <row r="152" spans="1:7" ht="50" customHeight="1">
       <c r="A152" s="42"/>
@@ -18719,6 +18824,9 @@
       </c>
       <c r="D405" s="29" t="s">
         <v>788</v>
+      </c>
+      <c r="E405" s="15" t="s">
+        <v>983</v>
       </c>
       <c r="G405" s="33" t="s">
         <v>917</v>
@@ -19282,16 +19390,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1765E8E-7B87-4E57-AE04-80D6CA061ADD}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1750c493-bee6-4013-b7a9-faed7d1eacd9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0fddf207-9565-4c1d-88a2-78ac3eb02019"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1750c493-bee6-4013-b7a9-faed7d1eacd9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0fddf207-9565-4c1d-88a2-78ac3eb02019"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>